<commit_message>
Added code to read data from SSB and other sources
There is now a file in reports that loads three datasets from SSB and one from EIA.gov. Also, some folder structures where changed, and some scripts were deprecated.
</commit_message>
<xml_diff>
--- a/ssb_data_sets.xlsx
+++ b/ssb_data_sets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="135" documentId="11_AD4DD024A17053AB440FF46D911D44685ADEDD9F" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{79FEEC16-15E3-4393-A339-88F40D4A87E4}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4470" yWindow="0" windowWidth="18570" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Arbeidsledige, etter kjønn og alder 1972 - 2018</t>
   </si>
@@ -152,14 +151,28 @@
   </si>
   <si>
     <t>Konsumprisindeks, historisk serie (2015=100) 1920M03 - 2018M12</t>
+  </si>
+  <si>
+    <t>EIA</t>
+  </si>
+  <si>
+    <t>Oljepriser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -187,9 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,20 +552,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -561,7 +576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -569,7 +584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -589,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -609,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -629,27 +644,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>1990</v>
       </c>
-      <c r="C7">
-        <v>2018</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -669,47 +684,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1992</v>
       </c>
-      <c r="C9">
-        <v>2018</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>1986</v>
       </c>
-      <c r="C10">
-        <v>2018</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -729,7 +744,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -749,7 +764,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -769,7 +784,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -789,7 +804,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -809,7 +824,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -829,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>